<commit_message>
fix CHL population (admin) issue and COL trust region
</commit_message>
<xml_diff>
--- a/input_data/admin_data/CHL/_clean/total-pos-CHL.xlsx
+++ b/input_data/admin_data/CHL/_clean/total-pos-CHL.xlsx
@@ -181,16 +181,16 @@
         <v>1.6156335E7</v>
       </c>
       <c r="F2" t="n">
-        <v>773954.5319734466</v>
+        <v>1471467.0078183615</v>
       </c>
       <c r="G2" t="n">
-        <v>0.6762153669133502</v>
+        <v>0.5648847340687104</v>
       </c>
       <c r="H2" t="n">
         <v>0.0</v>
       </c>
       <c r="I2" t="n">
-        <v>1595634.901762361</v>
+        <v>1602031.8886108703</v>
       </c>
     </row>
     <row r="3">
@@ -207,13 +207,13 @@
       <c r="E3"/>
       <c r="F3"/>
       <c r="G3" t="n">
-        <v>0.9686596619839833</v>
+        <v>0.9308043563097695</v>
       </c>
       <c r="H3" t="n">
         <v>5114502.0</v>
       </c>
       <c r="I3" t="n">
-        <v>7356709.603834595</v>
+        <v>7584770.396703399</v>
       </c>
     </row>
     <row r="4">
@@ -230,13 +230,13 @@
       <c r="E4"/>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>0.9942601462522286</v>
+        <v>0.9763434590827684</v>
       </c>
       <c r="H4" t="n">
         <v>1.136556E7</v>
       </c>
       <c r="I4" t="n">
-        <v>1.4796713017039765E7</v>
+        <v>1.4581862615942182E7</v>
       </c>
     </row>
     <row r="5">
@@ -253,13 +253,13 @@
       <c r="E5"/>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>0.998129031119991</v>
+        <v>0.9890600188718542</v>
       </c>
       <c r="H5" t="n">
         <v>1.89426E7</v>
       </c>
       <c r="I5" t="n">
-        <v>2.2926273003576458E7</v>
+        <v>2.219962427970983E7</v>
       </c>
     </row>
     <row r="6">
@@ -276,13 +276,13 @@
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6" t="n">
-        <v>0.9991475789527761</v>
+        <v>0.9942026455876286</v>
       </c>
       <c r="H6" t="n">
         <v>2.651964E7</v>
       </c>
       <c r="I6" t="n">
-        <v>3.0316829073444773E7</v>
+        <v>2.9232892592957396E7</v>
       </c>
     </row>
     <row r="7">
@@ -299,13 +299,13 @@
       <c r="E7"/>
       <c r="F7"/>
       <c r="G7" t="n">
-        <v>0.9994983391963586</v>
+        <v>0.9967634986523862</v>
       </c>
       <c r="H7" t="n">
         <v>3.409668E7</v>
       </c>
       <c r="I7" t="n">
-        <v>3.7852751461661644E7</v>
+        <v>3.71142816788097E7</v>
       </c>
     </row>
     <row r="8">
@@ -322,13 +322,13 @@
       <c r="E8"/>
       <c r="F8"/>
       <c r="G8" t="n">
-        <v>0.9997058738878588</v>
+        <v>0.998470135708377</v>
       </c>
       <c r="H8" t="n">
         <v>4.546224E7</v>
       </c>
       <c r="I8" t="n">
-        <v>4.694407274698825E7</v>
+        <v>4.70931617761739E7</v>
       </c>
     </row>
     <row r="9">
@@ -345,13 +345,13 @@
       <c r="E9"/>
       <c r="F9"/>
       <c r="G9" t="n">
-        <v>0.9997894324424444</v>
+        <v>0.9991392230973175</v>
       </c>
       <c r="H9" t="n">
         <v>5.68278E7</v>
       </c>
       <c r="I9" t="n">
-        <v>7.586315083585505E7</v>
+        <v>8.195127581173013E7</v>
       </c>
     </row>
   </sheetData>
@@ -411,16 +411,16 @@
         <v>1.78645995E7</v>
       </c>
       <c r="F2" t="n">
-        <v>1242820.0324924618</v>
+        <v>3285587.2091633086</v>
       </c>
       <c r="G2" t="n">
-        <v>0.6453248783998768</v>
+        <v>0.47876570084876513</v>
       </c>
       <c r="H2" t="n">
         <v>0.0</v>
       </c>
       <c r="I2" t="n">
-        <v>2515372.7213640036</v>
+        <v>2623889.2899430934</v>
       </c>
     </row>
     <row r="3">
@@ -437,13 +437,13 @@
       <c r="E3"/>
       <c r="F3"/>
       <c r="G3" t="n">
-        <v>0.9662396573737911</v>
+        <v>0.878330213895923</v>
       </c>
       <c r="H3" t="n">
         <v>6998076.0</v>
       </c>
       <c r="I3" t="n">
-        <v>1.0019939028425148E7</v>
+        <v>1.0460011337214043E7</v>
       </c>
     </row>
     <row r="4">
@@ -460,13 +460,13 @@
       <c r="E4"/>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>0.9947426193349591</v>
+        <v>0.9572380002137747</v>
       </c>
       <c r="H4" t="n">
         <v>1.555128E7</v>
       </c>
       <c r="I4" t="n">
-        <v>2.0309666180035412E7</v>
+        <v>1.995515507519471E7</v>
       </c>
     </row>
     <row r="5">
@@ -483,13 +483,13 @@
       <c r="E5"/>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>0.9985132608206526</v>
+        <v>0.979203452056118</v>
       </c>
       <c r="H5" t="n">
         <v>2.59188E7</v>
       </c>
       <c r="I5" t="n">
-        <v>3.1911224268339407E7</v>
+        <v>3.0370675719516642E7</v>
       </c>
     </row>
     <row r="6">
@@ -506,13 +506,13 @@
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6" t="n">
-        <v>0.9992937429131843</v>
+        <v>0.9880454079029312</v>
       </c>
       <c r="H6" t="n">
         <v>3.628632E7</v>
       </c>
       <c r="I6" t="n">
-        <v>4.214372496760815E7</v>
+        <v>3.994908170963806E7</v>
       </c>
     </row>
     <row r="7">
@@ -529,13 +529,13 @@
       <c r="E7"/>
       <c r="F7"/>
       <c r="G7" t="n">
-        <v>0.9995551537553361</v>
+        <v>0.9927922257647029</v>
       </c>
       <c r="H7" t="n">
         <v>4.665384E7</v>
       </c>
       <c r="I7" t="n">
-        <v>5.299156144504737E7</v>
+        <v>5.061660450614726E7</v>
       </c>
     </row>
     <row r="8">
@@ -552,13 +552,13 @@
       <c r="E8"/>
       <c r="F8"/>
       <c r="G8" t="n">
-        <v>0.9997222439831355</v>
+        <v>0.9963049829356656</v>
       </c>
       <c r="H8" t="n">
         <v>6.220512E7</v>
       </c>
       <c r="I8" t="n">
-        <v>6.619178430608356E7</v>
+        <v>6.342997986843106E7</v>
       </c>
     </row>
     <row r="9">
@@ -575,13 +575,13 @@
       <c r="E9"/>
       <c r="F9"/>
       <c r="G9" t="n">
-        <v>0.999801282978664</v>
+        <v>0.9978705931806644</v>
       </c>
       <c r="H9" t="n">
         <v>7.77564E7</v>
       </c>
       <c r="I9" t="n">
-        <v>1.1781713834866574E8</v>
+        <v>1.118603397638312E8</v>
       </c>
     </row>
   </sheetData>
@@ -641,16 +641,16 @@
         <v>1.8048518E7</v>
       </c>
       <c r="F2" t="n">
-        <v>1297225.4149316198</v>
+        <v>3511322.2800362553</v>
       </c>
       <c r="G2" t="n">
-        <v>0.6455750549712724</v>
+        <v>0.4732553664516943</v>
       </c>
       <c r="H2" t="n">
         <v>0.0</v>
       </c>
       <c r="I2" t="n">
-        <v>2634047.1323161656</v>
+        <v>2742302.5107261427</v>
       </c>
     </row>
     <row r="3">
@@ -667,13 +667,13 @@
       <c r="E3"/>
       <c r="F3"/>
       <c r="G3" t="n">
-        <v>0.9662023773918723</v>
+        <v>0.874651425673842</v>
       </c>
       <c r="H3" t="n">
         <v>7282710.0</v>
       </c>
       <c r="I3" t="n">
-        <v>1.0416473295811282E7</v>
+        <v>1.0881424000644643E7</v>
       </c>
     </row>
     <row r="4">
@@ -690,13 +690,13 @@
       <c r="E4"/>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>0.9947203975417815</v>
+        <v>0.9558061221425493</v>
       </c>
       <c r="H4" t="n">
         <v>1.61838E7</v>
       </c>
       <c r="I4" t="n">
-        <v>2.1109280875789437E7</v>
+        <v>2.0824035051397994E7</v>
       </c>
     </row>
     <row r="5">
@@ -713,13 +713,13 @@
       <c r="E5"/>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>0.9985362233065341</v>
+        <v>0.978614643041606</v>
       </c>
       <c r="H5" t="n">
         <v>2.6973E7</v>
       </c>
       <c r="I5" t="n">
-        <v>3.3225373546273332E7</v>
+        <v>3.15551466830572E7</v>
       </c>
     </row>
     <row r="6">
@@ -736,13 +736,13 @@
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6" t="n">
-        <v>0.999318004946445</v>
+        <v>0.9877198227577466</v>
       </c>
       <c r="H6" t="n">
         <v>3.77622E7</v>
       </c>
       <c r="I6" t="n">
-        <v>4.388799993117124E7</v>
+        <v>4.134209955142056E7</v>
       </c>
     </row>
     <row r="7">
@@ -759,13 +759,13 @@
       <c r="E7"/>
       <c r="F7"/>
       <c r="G7" t="n">
-        <v>0.9995681639899742</v>
+        <v>0.9925230426121413</v>
       </c>
       <c r="H7" t="n">
         <v>4.85514E7</v>
       </c>
       <c r="I7" t="n">
-        <v>5.5285165724980645E7</v>
+        <v>5.264239298865285E7</v>
       </c>
     </row>
     <row r="8">
@@ -782,13 +782,13 @@
       <c r="E8"/>
       <c r="F8"/>
       <c r="G8" t="n">
-        <v>0.9997327758434238</v>
+        <v>0.9960108636066407</v>
       </c>
       <c r="H8" t="n">
         <v>6.47352E7</v>
       </c>
       <c r="I8" t="n">
-        <v>6.904316401006845E7</v>
+        <v>6.56575612713272E7</v>
       </c>
     </row>
     <row r="9">
@@ -805,13 +805,13 @@
       <c r="E9"/>
       <c r="F9"/>
       <c r="G9" t="n">
-        <v>0.9998111202260485</v>
+        <v>0.9976973732690961</v>
       </c>
       <c r="H9" t="n">
         <v>8.0919E7</v>
       </c>
       <c r="I9" t="n">
-        <v>1.2498796102637285E8</v>
+        <v>1.1825578367482351E8</v>
       </c>
     </row>
   </sheetData>
@@ -871,16 +871,16 @@
         <v>1.8300725E7</v>
       </c>
       <c r="F2" t="n">
-        <v>1362021.2414222686</v>
+        <v>3658635.290172265</v>
       </c>
       <c r="G2" t="n">
-        <v>0.6427200561726379</v>
+        <v>0.46750617803393035</v>
       </c>
       <c r="H2" t="n">
         <v>0.0</v>
       </c>
       <c r="I2" t="n">
-        <v>2730108.0405918197</v>
+        <v>2835591.604773131</v>
       </c>
     </row>
     <row r="3">
@@ -897,13 +897,13 @@
       <c r="E3"/>
       <c r="F3"/>
       <c r="G3" t="n">
-        <v>0.9646135330704111</v>
+        <v>0.8723375166830822</v>
       </c>
       <c r="H3" t="n">
         <v>7481646.0</v>
       </c>
       <c r="I3" t="n">
-        <v>1.0687424193803985E7</v>
+        <v>1.1169404984355932E7</v>
       </c>
     </row>
     <row r="4">
@@ -920,13 +920,13 @@
       <c r="E4"/>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>0.9945524562551483</v>
+        <v>0.9552526470945824</v>
       </c>
       <c r="H4" t="n">
         <v>1.662588E7</v>
       </c>
       <c r="I4" t="n">
-        <v>2.1657572208319977E7</v>
+        <v>2.1400795929208297E7</v>
       </c>
     </row>
     <row r="5">
@@ -943,13 +943,13 @@
       <c r="E5"/>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>0.9985344842895568</v>
+        <v>0.978526260571644</v>
       </c>
       <c r="H5" t="n">
         <v>2.77098E7</v>
       </c>
       <c r="I5" t="n">
-        <v>3.4142707277689874E7</v>
+        <v>3.2408378383606467E7</v>
       </c>
     </row>
     <row r="6">
@@ -966,13 +966,13 @@
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6" t="n">
-        <v>0.9993376218701718</v>
+        <v>0.987629998265096</v>
       </c>
       <c r="H6" t="n">
         <v>3.879372E7</v>
       </c>
       <c r="I6" t="n">
-        <v>4.500871194510433E7</v>
+        <v>4.252900167424819E7</v>
       </c>
     </row>
     <row r="7">
@@ -989,13 +989,13 @@
       <c r="E7"/>
       <c r="F7"/>
       <c r="G7" t="n">
-        <v>0.9995801259239729</v>
+        <v>0.9924050549909907</v>
       </c>
       <c r="H7" t="n">
         <v>4.987764E7</v>
       </c>
       <c r="I7" t="n">
-        <v>5.6970328899390705E7</v>
+        <v>5.409395788325694E7</v>
       </c>
     </row>
     <row r="8">
@@ -1012,13 +1012,13 @@
       <c r="E8"/>
       <c r="F8"/>
       <c r="G8" t="n">
-        <v>0.9997401195854263</v>
+        <v>0.9959732742828494</v>
       </c>
       <c r="H8" t="n">
         <v>6.650352E7</v>
       </c>
       <c r="I8" t="n">
-        <v>7.121028443029065E7</v>
+        <v>6.747541985788348E7</v>
       </c>
     </row>
     <row r="9">
@@ -1035,13 +1035,13 @@
       <c r="E9"/>
       <c r="F9"/>
       <c r="G9" t="n">
-        <v>0.9998215371248953</v>
+        <v>0.9976705294462378</v>
       </c>
       <c r="H9" t="n">
         <v>8.31294E7</v>
       </c>
       <c r="I9" t="n">
-        <v>1.3312290393274614E8</v>
+        <v>1.2056582592518646E8</v>
       </c>
     </row>
   </sheetData>
@@ -1101,16 +1101,16 @@
         <v>1.8552932E7</v>
       </c>
       <c r="F2" t="n">
-        <v>1431930.8837916155</v>
+        <v>3870038.349771524</v>
       </c>
       <c r="G2" t="n">
-        <v>0.6512135655970711</v>
+        <v>0.46203640481191866</v>
       </c>
       <c r="H2" t="n">
         <v>0.0</v>
       </c>
       <c r="I2" t="n">
-        <v>2785508.327321361</v>
+        <v>2894885.5280024405</v>
       </c>
     </row>
     <row r="3">
@@ -1127,13 +1127,13 @@
       <c r="E3"/>
       <c r="F3"/>
       <c r="G3" t="n">
-        <v>0.9602915593071758</v>
+        <v>0.8674554512461965</v>
       </c>
       <c r="H3" t="n">
         <v>7609464.0</v>
       </c>
       <c r="I3" t="n">
-        <v>1.0922192388123658E7</v>
+        <v>1.1387059477224283E7</v>
       </c>
     </row>
     <row r="4">
@@ -1150,13 +1150,13 @@
       <c r="E4"/>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>0.9934078883057406</v>
+        <v>0.9538495586573594</v>
       </c>
       <c r="H4" t="n">
         <v>1.690992E7</v>
       </c>
       <c r="I4" t="n">
-        <v>2.1950824007972132E7</v>
+        <v>2.174412307966886E7</v>
       </c>
     </row>
     <row r="5">
@@ -1173,13 +1173,13 @@
       <c r="E5"/>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>0.998134472761502</v>
+        <v>0.9781913176849891</v>
       </c>
       <c r="H5" t="n">
         <v>2.81832E7</v>
       </c>
       <c r="I5" t="n">
-        <v>3.454541957542733E7</v>
+        <v>3.2902593283467546E7</v>
       </c>
     </row>
     <row r="6">
@@ -1196,13 +1196,13 @@
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6" t="n">
-        <v>0.9990793907938648</v>
+        <v>0.987420263276985</v>
       </c>
       <c r="H6" t="n">
         <v>3.945648E7</v>
       </c>
       <c r="I6" t="n">
-        <v>4.5919193048110545E7</v>
+        <v>4.323789983004427E7</v>
       </c>
     </row>
     <row r="7">
@@ -1219,13 +1219,13 @@
       <c r="E7"/>
       <c r="F7"/>
       <c r="G7" t="n">
-        <v>0.999376217193056</v>
+        <v>0.9920452465410858</v>
       </c>
       <c r="H7" t="n">
         <v>5.072976E7</v>
       </c>
       <c r="I7" t="n">
-        <v>5.818253537288825E7</v>
+        <v>5.4918134479413025E7</v>
       </c>
     </row>
     <row r="8">
@@ -1242,13 +1242,13 @@
       <c r="E8"/>
       <c r="F8"/>
       <c r="G8" t="n">
-        <v>0.9995678311115461</v>
+        <v>0.9955066401364485</v>
       </c>
       <c r="H8" t="n">
         <v>6.763968E7</v>
       </c>
       <c r="I8" t="n">
-        <v>1.1133382698008205E8</v>
+        <v>1.0896244796795504E8</v>
       </c>
     </row>
   </sheetData>
@@ -1308,16 +1308,16 @@
         <v>1.888368E7</v>
       </c>
       <c r="F2" t="n">
-        <v>1441629.726319768</v>
+        <v>4077068.3749480858</v>
       </c>
       <c r="G2" t="n">
-        <v>0.6466730531337113</v>
+        <v>0.45540397846182523</v>
       </c>
       <c r="H2" t="n">
         <v>0.0</v>
       </c>
       <c r="I2" t="n">
-        <v>2886418.0444340114</v>
+        <v>2999510.437243746</v>
       </c>
     </row>
     <row r="3">
@@ -1334,13 +1334,13 @@
       <c r="E3"/>
       <c r="F3"/>
       <c r="G3" t="n">
-        <v>0.9622435881141811</v>
+        <v>0.8638960732230159</v>
       </c>
       <c r="H3" t="n">
         <v>7833186.0</v>
       </c>
       <c r="I3" t="n">
-        <v>1.1238667164824773E7</v>
+        <v>1.1748281444795383E7</v>
       </c>
     </row>
     <row r="4">
@@ -1357,13 +1357,13 @@
       <c r="E4"/>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>0.994324040653093</v>
+        <v>0.9525272086796641</v>
       </c>
       <c r="H4" t="n">
         <v>1.740708E7</v>
       </c>
       <c r="I4" t="n">
-        <v>2.261438981643458E7</v>
+        <v>2.2355295363601692E7</v>
       </c>
     </row>
     <row r="5">
@@ -1380,13 +1380,13 @@
       <c r="E5"/>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>0.9986145708887251</v>
+        <v>0.9776674885403692</v>
       </c>
       <c r="H5" t="n">
         <v>2.90118E7</v>
       </c>
       <c r="I5" t="n">
-        <v>3.567108566797526E7</v>
+        <v>3.387389619045589E7</v>
       </c>
     </row>
     <row r="6">
@@ -1403,13 +1403,13 @@
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6" t="n">
-        <v>0.9993985282529676</v>
+        <v>0.9870517822797251</v>
       </c>
       <c r="H6" t="n">
         <v>4.061652E7</v>
       </c>
       <c r="I6" t="n">
-        <v>4.7160226411046565E7</v>
+        <v>4.449109112941603E7</v>
       </c>
     </row>
     <row r="7">
@@ -1426,13 +1426,13 @@
       <c r="E7"/>
       <c r="F7"/>
       <c r="G7" t="n">
-        <v>0.9996301038780576</v>
+        <v>0.9917963553714106</v>
       </c>
       <c r="H7" t="n">
         <v>5.222124E7</v>
       </c>
       <c r="I7" t="n">
-        <v>5.9832964243078806E7</v>
+        <v>5.6494216610647224E7</v>
       </c>
     </row>
     <row r="8">
@@ -1449,13 +1449,13 @@
       <c r="E8"/>
       <c r="F8"/>
       <c r="G8" t="n">
-        <v>0.9997734551739915</v>
+        <v>0.9954643374596477</v>
       </c>
       <c r="H8" t="n">
         <v>6.962832E7</v>
       </c>
       <c r="I8" t="n">
-        <v>1.135717212788602E8</v>
+        <v>1.1295297265600863E8</v>
       </c>
     </row>
   </sheetData>
@@ -1515,16 +1515,16 @@
         <v>1.9214428E7</v>
       </c>
       <c r="F2" t="n">
-        <v>1497825.106328016</v>
+        <v>4290358.911379947</v>
       </c>
       <c r="G2" t="n">
-        <v>0.6509250236332822</v>
+        <v>0.45314973727034713</v>
       </c>
       <c r="H2" t="n">
         <v>0.0</v>
       </c>
       <c r="I2" t="n">
-        <v>3021235.8149083387</v>
+        <v>3130947.6403722856</v>
       </c>
     </row>
     <row r="3">
@@ -1541,13 +1541,13 @@
       <c r="E3"/>
       <c r="F3"/>
       <c r="G3" t="n">
-        <v>0.961346754636672</v>
+        <v>0.8594570184446813</v>
       </c>
       <c r="H3" t="n">
         <v>8038926.0</v>
       </c>
       <c r="I3" t="n">
-        <v>1.154565658423482E7</v>
+        <v>1.2062663834026156E7</v>
       </c>
     </row>
     <row r="4">
@@ -1564,13 +1564,13 @@
       <c r="E4"/>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>0.9941811955057939</v>
+        <v>0.9513523899852756</v>
       </c>
       <c r="H4" t="n">
         <v>1.786428E7</v>
       </c>
       <c r="I4" t="n">
-        <v>2.3255846196233004E7</v>
+        <v>2.295538251088929E7</v>
       </c>
     </row>
     <row r="5">
@@ -1587,13 +1587,13 @@
       <c r="E5"/>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>0.9985683154346306</v>
+        <v>0.9775300623052635</v>
       </c>
       <c r="H5" t="n">
         <v>2.97738E7</v>
       </c>
       <c r="I5" t="n">
-        <v>3.6647912808426745E7</v>
+        <v>3.475211080265494E7</v>
       </c>
     </row>
     <row r="6">
@@ -1610,13 +1610,13 @@
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6" t="n">
-        <v>0.9993708373728325</v>
+        <v>0.987171671204576</v>
       </c>
       <c r="H6" t="n">
         <v>4.168332E7</v>
       </c>
       <c r="I6" t="n">
-        <v>4.842033780094835E7</v>
+        <v>4.565587598131721E7</v>
       </c>
     </row>
     <row r="7">
@@ -1633,13 +1633,13 @@
       <c r="E7"/>
       <c r="F7"/>
       <c r="G7" t="n">
-        <v>0.9996064415760907</v>
+        <v>0.9918613242090787</v>
       </c>
       <c r="H7" t="n">
         <v>5.359284E7</v>
       </c>
       <c r="I7" t="n">
-        <v>6.133259549953238E7</v>
+        <v>5.795885798708902E7</v>
       </c>
     </row>
     <row r="8">
@@ -1656,13 +1656,13 @@
       <c r="E8"/>
       <c r="F8"/>
       <c r="G8" t="n">
-        <v>0.9997586188878482</v>
+        <v>0.9953999671496856</v>
       </c>
       <c r="H8" t="n">
         <v>7.145712E7</v>
       </c>
       <c r="I8" t="n">
-        <v>1.1887538045479406E8</v>
+        <v>1.205509763958786E8</v>
       </c>
     </row>
   </sheetData>
@@ -1722,16 +1722,16 @@
         <v>1.9545176E7</v>
       </c>
       <c r="F2" t="n">
-        <v>1422022.958431771</v>
+        <v>4001451.3044119664</v>
       </c>
       <c r="G2" t="n">
-        <v>0.6645241772189721</v>
+        <v>0.47230815419620675</v>
       </c>
       <c r="H2" t="n">
         <v>0.0</v>
       </c>
       <c r="I2" t="n">
-        <v>2989615.303410954</v>
+        <v>3134480.941612259</v>
       </c>
     </row>
     <row r="3">
@@ -1748,13 +1748,13 @@
       <c r="E3"/>
       <c r="F3"/>
       <c r="G3" t="n">
-        <v>0.9650374598826841</v>
+        <v>0.8704249068926266</v>
       </c>
       <c r="H3" t="n">
         <v>8266698.0</v>
       </c>
       <c r="I3" t="n">
-        <v>1.1892208101905433E7</v>
+        <v>1.2431143892807288E7</v>
       </c>
     </row>
     <row r="4">
@@ -1771,13 +1771,13 @@
       <c r="E4"/>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>0.9944014318418007</v>
+        <v>0.9559488233823016</v>
       </c>
       <c r="H4" t="n">
         <v>1.837044E7</v>
       </c>
       <c r="I4" t="n">
-        <v>2.3872728158913646E7</v>
+        <v>2.3930534850447875E7</v>
       </c>
     </row>
     <row r="5">
@@ -1794,13 +1794,13 @@
       <c r="E5"/>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>0.9986700043018287</v>
+        <v>0.9798714526796791</v>
       </c>
       <c r="H5" t="n">
         <v>3.06174E7</v>
       </c>
       <c r="I5" t="n">
-        <v>3.7671132303679235E7</v>
+        <v>3.572633521871039E7</v>
       </c>
     </row>
     <row r="6">
@@ -1817,13 +1817,13 @@
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6" t="n">
-        <v>0.9994408850552177</v>
+        <v>0.989162543228058</v>
       </c>
       <c r="H6" t="n">
         <v>4.286436E7</v>
       </c>
       <c r="I6" t="n">
-        <v>4.972913411746434E7</v>
+        <v>4.710067646536338E7</v>
       </c>
     </row>
     <row r="7">
@@ -1840,13 +1840,13 @@
       <c r="E7"/>
       <c r="F7"/>
       <c r="G7" t="n">
-        <v>0.9996728604541602</v>
+        <v>0.9934771116924197</v>
       </c>
       <c r="H7" t="n">
         <v>5.511132E7</v>
       </c>
       <c r="I7" t="n">
-        <v>6.303938409100993E7</v>
+        <v>5.9812873660499424E7</v>
       </c>
     </row>
     <row r="8">
@@ -1863,13 +1863,13 @@
       <c r="E8"/>
       <c r="F8"/>
       <c r="G8" t="n">
-        <v>0.9998067042220546</v>
+        <v>0.9964965779791392</v>
       </c>
       <c r="H8" t="n">
         <v>7.348176E7</v>
       </c>
       <c r="I8" t="n">
-        <v>9.883594056464191E7</v>
+        <v>9.27354684031255E7</v>
       </c>
     </row>
     <row r="9">
@@ -1886,13 +1886,13 @@
       <c r="E9"/>
       <c r="F9"/>
       <c r="G9" t="n">
-        <v>0.9999731903156053</v>
+        <v>0.9995871103949128</v>
       </c>
       <c r="H9" t="n">
         <v>1.8982788E8</v>
       </c>
       <c r="I9" t="n">
-        <v>2.6224812946743298E8</v>
+        <v>2.7988078973654926E8</v>
       </c>
     </row>
   </sheetData>
@@ -1952,16 +1952,16 @@
         <v>1.97118745E7</v>
       </c>
       <c r="F2" t="n">
-        <v>1629050.4417849144</v>
+        <v>4644475.5531022055</v>
       </c>
       <c r="G2" t="n">
-        <v>0.6581280993849672</v>
+        <v>0.4616286746346726</v>
       </c>
       <c r="H2" t="n">
         <v>0.0</v>
       </c>
       <c r="I2" t="n">
-        <v>3303028.767777756</v>
+        <v>3450978.569739974</v>
       </c>
     </row>
     <row r="3">
@@ -1978,13 +1978,13 @@
       <c r="E3"/>
       <c r="F3"/>
       <c r="G3" t="n">
-        <v>0.9606316994357893</v>
+        <v>0.8598693391640658</v>
       </c>
       <c r="H3" t="n">
         <v>8775702.0</v>
       </c>
       <c r="I3" t="n">
-        <v>1.2567085866377342E7</v>
+        <v>1.3201523719390333E7</v>
       </c>
     </row>
     <row r="4">
@@ -2001,13 +2001,13 @@
       <c r="E4"/>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>0.9936325183076831</v>
+        <v>0.9515215562071482</v>
       </c>
       <c r="H4" t="n">
         <v>1.950156E7</v>
       </c>
       <c r="I4" t="n">
-        <v>2.5250949759708792E7</v>
+        <v>2.5560057311019223E7</v>
       </c>
     </row>
     <row r="5">
@@ -2024,13 +2024,13 @@
       <c r="E5"/>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>0.9983329337856732</v>
+        <v>0.976440850412273</v>
       </c>
       <c r="H5" t="n">
         <v>3.25026E7</v>
       </c>
       <c r="I5" t="n">
-        <v>3.965981843916193E7</v>
+        <v>3.789300388917709E7</v>
       </c>
     </row>
     <row r="6">
@@ -2047,13 +2047,13 @@
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6" t="n">
-        <v>0.999271099255426</v>
+        <v>0.986866850232838</v>
       </c>
       <c r="H6" t="n">
         <v>4.550364E7</v>
       </c>
       <c r="I6" t="n">
-        <v>5.281747278947407E7</v>
+        <v>4.9823978044866905E7</v>
       </c>
     </row>
     <row r="7">
@@ -2070,13 +2070,13 @@
       <c r="E7"/>
       <c r="F7"/>
       <c r="G7" t="n">
-        <v>0.9995702590334572</v>
+        <v>0.9919520084201023</v>
       </c>
       <c r="H7" t="n">
         <v>5.850468E7</v>
       </c>
       <c r="I7" t="n">
-        <v>6.698173340873455E7</v>
+        <v>6.3269540051289186E7</v>
       </c>
     </row>
     <row r="8">
@@ -2093,13 +2093,13 @@
       <c r="E8"/>
       <c r="F8"/>
       <c r="G8" t="n">
-        <v>0.9997601953076558</v>
+        <v>0.9957050254150106</v>
       </c>
       <c r="H8" t="n">
         <v>7.800624E7</v>
       </c>
       <c r="I8" t="n">
-        <v>1.0398715746292216E8</v>
+        <v>9.772527360991237E7</v>
       </c>
     </row>
     <row r="9">
@@ -2116,13 +2116,13 @@
       <c r="E9"/>
       <c r="F9"/>
       <c r="G9" t="n">
-        <v>0.9999762072348827</v>
+        <v>0.9994975110053588</v>
       </c>
       <c r="H9" t="n">
         <v>2.0151612E8</v>
       </c>
       <c r="I9" t="n">
-        <v>3.4738316904478085E8</v>
+        <v>3.3186684295864373E8</v>
       </c>
     </row>
   </sheetData>
@@ -2182,16 +2182,16 @@
         <v>1.9878573E7</v>
       </c>
       <c r="F2" t="n">
-        <v>1972919.6192587845</v>
+        <v>5414527.274697046</v>
       </c>
       <c r="G2" t="n">
-        <v>0.6335948762519321</v>
+        <v>0.4286159273102752</v>
       </c>
       <c r="H2" t="n">
         <v>0.0</v>
       </c>
       <c r="I2" t="n">
-        <v>3874255.251136734</v>
+        <v>4047733.2194742034</v>
       </c>
     </row>
     <row r="3">
@@ -2208,13 +2208,13 @@
       <c r="E3"/>
       <c r="F3"/>
       <c r="G3" t="n">
-        <v>0.9591259392713953</v>
+        <v>0.8530505182640625</v>
       </c>
       <c r="H3" t="n">
         <v>9907434.0</v>
       </c>
       <c r="I3" t="n">
-        <v>1.4140686874502946E7</v>
+        <v>1.4831504769392628E7</v>
       </c>
     </row>
     <row r="4">
@@ -2231,13 +2231,13 @@
       <c r="E4"/>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>0.9943628247359607</v>
+        <v>0.9511587174793683</v>
       </c>
       <c r="H4" t="n">
         <v>2.201652E7</v>
       </c>
       <c r="I4" t="n">
-        <v>2.856366701731188E7</v>
+        <v>2.8285742675048497E7</v>
       </c>
     </row>
     <row r="5">
@@ -2254,13 +2254,13 @@
       <c r="E5"/>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>0.9986230902992886</v>
+        <v>0.9782664983044809</v>
       </c>
       <c r="H5" t="n">
         <v>3.66942E7</v>
       </c>
       <c r="I5" t="n">
-        <v>4.498258516089623E7</v>
+        <v>4.284533436551678E7</v>
       </c>
     </row>
     <row r="6">
@@ -2277,13 +2277,13 @@
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6" t="n">
-        <v>0.9994007115098251</v>
+        <v>0.9881426096329953</v>
       </c>
       <c r="H6" t="n">
         <v>5.137188E7</v>
       </c>
       <c r="I6" t="n">
-        <v>5.964520370105975E7</v>
+        <v>5.650297354972678E7</v>
       </c>
     </row>
     <row r="7">
@@ -2300,13 +2300,13 @@
       <c r="E7"/>
       <c r="F7"/>
       <c r="G7" t="n">
-        <v>0.9996417750912</v>
+        <v>0.9928250886016818</v>
       </c>
       <c r="H7" t="n">
         <v>6.604956E7</v>
       </c>
       <c r="I7" t="n">
-        <v>7.567312782079098E7</v>
+        <v>7.170994991986142E7</v>
       </c>
     </row>
     <row r="8">
@@ -2323,13 +2323,13 @@
       <c r="E8"/>
       <c r="F8"/>
       <c r="G8" t="n">
-        <v>0.9997920373861846</v>
+        <v>0.9960944882713664</v>
       </c>
       <c r="H8" t="n">
         <v>8.806608E7</v>
       </c>
       <c r="I8" t="n">
-        <v>1.2072365504120879E8</v>
+        <v>1.1230967966690683E8</v>
       </c>
     </row>
     <row r="9">
@@ -2346,13 +2346,13 @@
       <c r="E9"/>
       <c r="F9"/>
       <c r="G9" t="n">
-        <v>0.9999756018704159</v>
+        <v>0.999509773664337</v>
       </c>
       <c r="H9" t="n">
         <v>2.2750404E8</v>
       </c>
       <c r="I9" t="n">
-        <v>3.638609305887323E8</v>
+        <v>3.446081109230784E8</v>
       </c>
     </row>
   </sheetData>
@@ -2412,16 +2412,16 @@
         <v>1.9878573E7</v>
       </c>
       <c r="F2" t="n">
-        <v>2302255.28722011</v>
+        <v>5875212.569846148</v>
       </c>
       <c r="G2" t="n">
-        <v>0.6357270715558908</v>
+        <v>0.43963175827560663</v>
       </c>
       <c r="H2" t="n">
         <v>0.0</v>
       </c>
       <c r="I2" t="n">
-        <v>4314621.371012199</v>
+        <v>4416819.081287886</v>
       </c>
     </row>
     <row r="3">
@@ -2438,13 +2438,13 @@
       <c r="E3"/>
       <c r="F3"/>
       <c r="G3" t="n">
-        <v>0.9485694471127278</v>
+        <v>0.8459803427539794</v>
       </c>
       <c r="H3" t="n">
         <v>1.0402992E7</v>
       </c>
       <c r="I3" t="n">
-        <v>1.4921901025012618E7</v>
+        <v>1.5607865081082175E7</v>
       </c>
     </row>
     <row r="4">
@@ -2461,13 +2461,13 @@
       <c r="E4"/>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>0.99236746017936</v>
+        <v>0.9482767198631411</v>
       </c>
       <c r="H4" t="n">
         <v>2.311776E7</v>
       </c>
       <c r="I4" t="n">
-        <v>2.9904024936020393E7</v>
+        <v>2.972509148657573E7</v>
       </c>
     </row>
     <row r="5">
@@ -2484,13 +2484,13 @@
       <c r="E5"/>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>0.9981425729100374</v>
+        <v>0.9767779608727447</v>
       </c>
       <c r="H5" t="n">
         <v>3.85296E7</v>
       </c>
       <c r="I5" t="n">
-        <v>4.714219459319152E7</v>
+        <v>4.494224270705617E7</v>
       </c>
     </row>
     <row r="6">
@@ -2507,13 +2507,13 @@
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6" t="n">
-        <v>0.9991887244622639</v>
+        <v>0.9872546183269795</v>
       </c>
       <c r="H6" t="n">
         <v>5.394144E7</v>
       </c>
       <c r="I6" t="n">
-        <v>6.2913048340841986E7</v>
+        <v>5.90702654841964E7</v>
       </c>
     </row>
     <row r="7">
@@ -2530,13 +2530,13 @@
       <c r="E7"/>
       <c r="F7"/>
       <c r="G7" t="n">
-        <v>0.9995053467872166</v>
+        <v>0.9922773128634536</v>
       </c>
       <c r="H7" t="n">
         <v>6.935328E7</v>
       </c>
       <c r="I7" t="n">
-        <v>7.912827820589146E7</v>
+        <v>7.496738926672728E7</v>
       </c>
     </row>
     <row r="8">
@@ -2553,13 +2553,13 @@
       <c r="E8"/>
       <c r="F8"/>
       <c r="G8" t="n">
-        <v>0.999703650760042</v>
+        <v>0.9958301332796876</v>
       </c>
       <c r="H8" t="n">
         <v>9.247104E7</v>
       </c>
       <c r="I8" t="n">
-        <v>1.2290747650421886E8</v>
+        <v>1.171935740177113E8</v>
       </c>
     </row>
     <row r="9">
@@ -2576,13 +2576,13 @@
       <c r="E9"/>
       <c r="F9"/>
       <c r="G9" t="n">
-        <v>0.9999726338505284</v>
+        <v>0.999503535792031</v>
       </c>
       <c r="H9" t="n">
         <v>2.3888352E8</v>
       </c>
       <c r="I9" t="n">
-        <v>3.004118728601765E8</v>
+        <v>3.46919505294065E8</v>
       </c>
     </row>
   </sheetData>
@@ -2642,16 +2642,16 @@
         <v>1.641461E7</v>
       </c>
       <c r="F2" t="n">
-        <v>829291.6050351905</v>
+        <v>1590792.9488749744</v>
       </c>
       <c r="G2" t="n">
-        <v>0.6661781790733986</v>
+        <v>0.5526031383017933</v>
       </c>
       <c r="H2" t="n">
         <v>0.0</v>
       </c>
       <c r="I2" t="n">
-        <v>1663438.1195051253</v>
+        <v>1670623.2263330012</v>
       </c>
     </row>
     <row r="3">
@@ -2668,13 +2668,13 @@
       <c r="E3"/>
       <c r="F3"/>
       <c r="G3" t="n">
-        <v>0.9671715014855669</v>
+        <v>0.9267414212095201</v>
       </c>
       <c r="H3" t="n">
         <v>5217372.0</v>
       </c>
       <c r="I3" t="n">
-        <v>7495348.844129017</v>
+        <v>7737922.871308645</v>
       </c>
     </row>
     <row r="4">
@@ -2691,13 +2691,13 @@
       <c r="E4"/>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>0.9941243197371122</v>
+        <v>0.9747010742259488</v>
       </c>
       <c r="H4" t="n">
         <v>1.159416E7</v>
       </c>
       <c r="I4" t="n">
-        <v>1.5057161351025334E7</v>
+        <v>1.4845312592525424E7</v>
       </c>
     </row>
     <row r="5">
@@ -2714,13 +2714,13 @@
       <c r="E5"/>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>0.9980144517597433</v>
+        <v>0.9879796717680164</v>
       </c>
       <c r="H5" t="n">
         <v>1.93236E7</v>
       </c>
       <c r="I5" t="n">
-        <v>2.3505298690950688E7</v>
+        <v>2.266256486397674E7</v>
       </c>
     </row>
     <row r="6">
@@ -2737,13 +2737,13 @@
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6" t="n">
-        <v>0.9989992451846251</v>
+        <v>0.9933682859355172</v>
       </c>
       <c r="H6" t="n">
         <v>2.705304E7</v>
       </c>
       <c r="I6" t="n">
-        <v>3.0734338038231693E7</v>
+        <v>2.9744082129487157E7</v>
       </c>
     </row>
     <row r="7">
@@ -2760,13 +2760,13 @@
       <c r="E7"/>
       <c r="F7"/>
       <c r="G7" t="n">
-        <v>0.9994383661871954</v>
+        <v>0.9963863290081214</v>
       </c>
       <c r="H7" t="n">
         <v>3.478248E7</v>
       </c>
       <c r="I7" t="n">
-        <v>3.831575498667861E7</v>
+        <v>3.7550872242191315E7</v>
       </c>
     </row>
     <row r="8">
@@ -2783,13 +2783,13 @@
       <c r="E8"/>
       <c r="F8"/>
       <c r="G8" t="n">
-        <v>0.9996763249324839</v>
+        <v>0.9983322783788344</v>
       </c>
       <c r="H8" t="n">
         <v>4.637664E7</v>
       </c>
       <c r="I8" t="n">
-        <v>4.7949430760116786E7</v>
+        <v>4.766804062825557E7</v>
       </c>
     </row>
     <row r="9">
@@ -2806,13 +2806,13 @@
       <c r="E9"/>
       <c r="F9"/>
       <c r="G9" t="n">
-        <v>0.9997598480865522</v>
+        <v>0.9990697311724128</v>
       </c>
       <c r="H9" t="n">
         <v>5.79708E7</v>
       </c>
       <c r="I9" t="n">
-        <v>7.597817681049928E7</v>
+        <v>8.320396100621802E7</v>
       </c>
     </row>
   </sheetData>
@@ -2872,16 +2872,16 @@
         <v>1.6594148E7</v>
       </c>
       <c r="F2" t="n">
-        <v>936786.3039852418</v>
+        <v>1795294.5108248428</v>
       </c>
       <c r="G2" t="n">
-        <v>0.6553459086902202</v>
+        <v>0.5408280075602556</v>
       </c>
       <c r="H2" t="n">
         <v>0.0</v>
       </c>
       <c r="I2" t="n">
-        <v>1810389.555427528</v>
+        <v>1819127.160527744</v>
       </c>
     </row>
     <row r="3">
@@ -2898,13 +2898,13 @@
       <c r="E3"/>
       <c r="F3"/>
       <c r="G3" t="n">
-        <v>0.9644274596080498</v>
+        <v>0.9213922884139638</v>
       </c>
       <c r="H3" t="n">
         <v>5543964.0</v>
       </c>
       <c r="I3" t="n">
-        <v>7966267.37176211</v>
+        <v>8220306.473795203</v>
       </c>
     </row>
     <row r="4">
@@ -2921,13 +2921,13 @@
       <c r="E4"/>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>0.9937574378630346</v>
+        <v>0.9727978200507793</v>
       </c>
       <c r="H4" t="n">
         <v>1.231992E7</v>
       </c>
       <c r="I4" t="n">
-        <v>1.5998935308415784E7</v>
+        <v>1.5775183211790984E7</v>
       </c>
     </row>
     <row r="5">
@@ -2944,13 +2944,13 @@
       <c r="E5"/>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>0.9979152891730265</v>
+        <v>0.986926716575024</v>
       </c>
       <c r="H5" t="n">
         <v>2.05332E7</v>
       </c>
       <c r="I5" t="n">
-        <v>2.492016140536585E7</v>
+        <v>2.3986874614445746E7</v>
       </c>
     </row>
     <row r="6">
@@ -2967,13 +2967,13 @@
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6" t="n">
-        <v>0.9989889206725167</v>
+        <v>0.9929825261290908</v>
       </c>
       <c r="H6" t="n">
         <v>2.874648E7</v>
       </c>
       <c r="I6" t="n">
-        <v>3.2773551353857342E7</v>
+        <v>3.1600861569078356E7</v>
       </c>
     </row>
     <row r="7">
@@ -2990,13 +2990,13 @@
       <c r="E7"/>
       <c r="F7"/>
       <c r="G7" t="n">
-        <v>0.9993983421143405</v>
+        <v>0.9961148351816556</v>
       </c>
       <c r="H7" t="n">
         <v>3.695976E7</v>
       </c>
       <c r="I7" t="n">
-        <v>4.0954326369429685E7</v>
+        <v>3.9981638739502326E7</v>
       </c>
     </row>
     <row r="8">
@@ -3013,13 +3013,13 @@
       <c r="E8"/>
       <c r="F8"/>
       <c r="G8" t="n">
-        <v>0.9996347507567126</v>
+        <v>0.9981695354289958</v>
       </c>
       <c r="H8" t="n">
         <v>4.927968E7</v>
       </c>
       <c r="I8" t="n">
-        <v>5.107394345343609E7</v>
+        <v>5.073123386384816E7</v>
       </c>
     </row>
     <row r="9">
@@ -3036,13 +3036,13 @@
       <c r="E9"/>
       <c r="F9"/>
       <c r="G9" t="n">
-        <v>0.9997309895030465</v>
+        <v>0.9989786760971398</v>
       </c>
       <c r="H9" t="n">
         <v>6.15996E7</v>
       </c>
       <c r="I9" t="n">
-        <v>8.284485502308005E7</v>
+        <v>8.822072850337543E7</v>
       </c>
     </row>
   </sheetData>
@@ -3102,16 +3102,16 @@
         <v>1.6773686E7</v>
       </c>
       <c r="F2" t="n">
-        <v>1045921.0823813769</v>
+        <v>2010612.8556716999</v>
       </c>
       <c r="G2" t="n">
-        <v>0.6461846251324843</v>
+        <v>0.5296808346120226</v>
       </c>
       <c r="H2" t="n">
         <v>0.0</v>
       </c>
       <c r="I2" t="n">
-        <v>1991826.2670669905</v>
+        <v>2008124.2608737485</v>
       </c>
     </row>
     <row r="3">
@@ -3128,13 +3128,13 @@
       <c r="E3"/>
       <c r="F3"/>
       <c r="G3" t="n">
-        <v>0.9645699818155652</v>
+        <v>0.9200633659173064</v>
       </c>
       <c r="H3" t="n">
         <v>6099624.0</v>
       </c>
       <c r="I3" t="n">
-        <v>8755407.647127043</v>
+        <v>9040650.462324321</v>
       </c>
     </row>
     <row r="4">
@@ -3151,13 +3151,13 @@
       <c r="E4"/>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>0.9938622912101729</v>
+        <v>0.9724718228301161</v>
       </c>
       <c r="H4" t="n">
         <v>1.355472E7</v>
       </c>
       <c r="I4" t="n">
-        <v>1.7590336831311453E7</v>
+        <v>1.735224749661529E7</v>
       </c>
     </row>
     <row r="5">
@@ -3174,13 +3174,13 @@
       <c r="E5"/>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>0.9979993067713322</v>
+        <v>0.9870244977758615</v>
       </c>
       <c r="H5" t="n">
         <v>2.25912E7</v>
       </c>
       <c r="I5" t="n">
-        <v>2.735782536068666E7</v>
+        <v>2.634893509949855E7</v>
       </c>
     </row>
     <row r="6">
@@ -3197,13 +3197,13 @@
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6" t="n">
-        <v>0.9990218607883801</v>
+        <v>0.9931516543233252</v>
       </c>
       <c r="H6" t="n">
         <v>3.162768E7</v>
       </c>
       <c r="I6" t="n">
-        <v>3.6130863614274494E7</v>
+        <v>3.476481213389001E7</v>
       </c>
     </row>
     <row r="7">
@@ -3220,13 +3220,13 @@
       <c r="E7"/>
       <c r="F7"/>
       <c r="G7" t="n">
-        <v>0.9993993568259236</v>
+        <v>0.9961390120215676</v>
       </c>
       <c r="H7" t="n">
         <v>4.066416E7</v>
       </c>
       <c r="I7" t="n">
-        <v>4.5181405984308295E7</v>
+        <v>4.398278074201012E7</v>
       </c>
     </row>
     <row r="8">
@@ -3243,13 +3243,13 @@
       <c r="E8"/>
       <c r="F8"/>
       <c r="G8" t="n">
-        <v>0.9996229808999644</v>
+        <v>0.9981585442817995</v>
       </c>
       <c r="H8" t="n">
         <v>5.421888E7</v>
       </c>
       <c r="I8" t="n">
-        <v>5.609052991530711E7</v>
+        <v>5.575909971380116E7</v>
       </c>
     </row>
     <row r="9">
@@ -3266,13 +3266,13 @@
       <c r="E9"/>
       <c r="F9"/>
       <c r="G9" t="n">
-        <v>0.999719262659382</v>
+        <v>0.9989680860843586</v>
       </c>
       <c r="H9" t="n">
         <v>6.77736E7</v>
       </c>
       <c r="I9" t="n">
-        <v>9.046499446848875E7</v>
+        <v>9.795886878244478E7</v>
       </c>
     </row>
   </sheetData>
@@ -3332,16 +3332,16 @@
         <v>1.6953224E7</v>
       </c>
       <c r="F2" t="n">
-        <v>1063147.8219711725</v>
+        <v>2049429.5099458704</v>
       </c>
       <c r="G2" t="n">
-        <v>0.6498988039089202</v>
+        <v>0.5323491272220553</v>
       </c>
       <c r="H2" t="n">
         <v>0.0</v>
       </c>
       <c r="I2" t="n">
-        <v>1979525.507205111</v>
+        <v>1989381.300836915</v>
       </c>
     </row>
     <row r="3">
@@ -3358,13 +3358,13 @@
       <c r="E3"/>
       <c r="F3"/>
       <c r="G3" t="n">
-        <v>0.9607659876375136</v>
+        <v>0.9146805351005802</v>
       </c>
       <c r="H3" t="n">
         <v>5971806.0</v>
       </c>
       <c r="I3" t="n">
-        <v>8607969.23136768</v>
+        <v>8873586.171530778</v>
       </c>
     </row>
     <row r="4">
@@ -3381,13 +3381,13 @@
       <c r="E4"/>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>0.9931897909211841</v>
+        <v>0.9706006951834059</v>
       </c>
       <c r="H4" t="n">
         <v>1.327068E7</v>
       </c>
       <c r="I4" t="n">
-        <v>1.7202020542037807E7</v>
+        <v>1.697567925646894E7</v>
       </c>
     </row>
     <row r="5">
@@ -3404,13 +3404,13 @@
       <c r="E5"/>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>0.9977808940647513</v>
+        <v>0.9859032122739604</v>
       </c>
       <c r="H5" t="n">
         <v>2.21178E7</v>
       </c>
       <c r="I5" t="n">
-        <v>2.6570026082832064E7</v>
+        <v>2.5766338371021293E7</v>
       </c>
     </row>
     <row r="6">
@@ -3427,13 +3427,13 @@
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6" t="n">
-        <v>0.9989097059060861</v>
+        <v>0.9922486130071778</v>
       </c>
       <c r="H6" t="n">
         <v>3.096492E7</v>
       </c>
       <c r="I6" t="n">
-        <v>3.541921035361429E7</v>
+        <v>3.39517260217948E7</v>
       </c>
     </row>
     <row r="7">
@@ -3450,13 +3450,13 @@
       <c r="E7"/>
       <c r="F7"/>
       <c r="G7" t="n">
-        <v>0.9993083321496843</v>
+        <v>0.9956074431624333</v>
       </c>
       <c r="H7" t="n">
         <v>3.981204E7</v>
       </c>
       <c r="I7" t="n">
-        <v>4.4390756595598795E7</v>
+        <v>4.2967784949911036E7</v>
       </c>
     </row>
     <row r="8">
@@ -3473,13 +3473,13 @@
       <c r="E8"/>
       <c r="F8"/>
       <c r="G8" t="n">
-        <v>0.999574299260129</v>
+        <v>0.9979783786258001</v>
       </c>
       <c r="H8" t="n">
         <v>5.308272E7</v>
       </c>
       <c r="I8" t="n">
-        <v>5.528604150634277E7</v>
+        <v>5.4111730342896946E7</v>
       </c>
     </row>
     <row r="9">
@@ -3496,13 +3496,13 @@
       <c r="E9"/>
       <c r="F9"/>
       <c r="G9" t="n">
-        <v>0.9996812995569456</v>
+        <v>0.9988748452801662</v>
       </c>
       <c r="H9" t="n">
         <v>6.63534E7</v>
       </c>
       <c r="I9" t="n">
-        <v>8.743401668916781E7</v>
+        <v>9.325343689553966E7</v>
       </c>
     </row>
   </sheetData>
@@ -3562,16 +3562,16 @@
         <v>1.714104E7</v>
       </c>
       <c r="F2" t="n">
-        <v>1159140.1563719339</v>
+        <v>2246976.0997764645</v>
       </c>
       <c r="G2" t="n">
-        <v>0.6401140770921718</v>
+        <v>0.5184649239486052</v>
       </c>
       <c r="H2" t="n">
         <v>0.0</v>
       </c>
       <c r="I2" t="n">
-        <v>2062135.057226786</v>
+        <v>2072043.485700192</v>
       </c>
     </row>
     <row r="3">
@@ -3588,13 +3588,13 @@
       <c r="E3"/>
       <c r="F3"/>
       <c r="G3" t="n">
-        <v>0.9565615038527417</v>
+        <v>0.9067410728870594</v>
       </c>
       <c r="H3" t="n">
         <v>6092010.0</v>
       </c>
       <c r="I3" t="n">
-        <v>8782578.259847669</v>
+        <v>9075493.593378935</v>
       </c>
     </row>
     <row r="4">
@@ -3611,13 +3611,13 @@
       <c r="E4"/>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>0.992438673499391</v>
+        <v>0.9676496875335452</v>
       </c>
       <c r="H4" t="n">
         <v>1.35378E7</v>
       </c>
       <c r="I4" t="n">
-        <v>1.7430230291540943E7</v>
+        <v>1.727481001488742E7</v>
       </c>
     </row>
     <row r="5">
@@ -3634,13 +3634,13 @@
       <c r="E5"/>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>0.9976163640012508</v>
+        <v>0.9845696643844247</v>
       </c>
       <c r="H5" t="n">
         <v>2.2563E7</v>
       </c>
       <c r="I5" t="n">
-        <v>2.714201045221589E7</v>
+        <v>2.6227649542412303E7</v>
       </c>
     </row>
     <row r="6">
@@ -3657,13 +3657,13 @@
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6" t="n">
-        <v>0.9988408521303258</v>
+        <v>0.9915555298861679</v>
       </c>
       <c r="H6" t="n">
         <v>3.15882E7</v>
       </c>
       <c r="I6" t="n">
-        <v>3.646637108732629E7</v>
+        <v>3.453794707980371E7</v>
       </c>
     </row>
     <row r="7">
@@ -3680,13 +3680,13 @@
       <c r="E7"/>
       <c r="F7"/>
       <c r="G7" t="n">
-        <v>0.999270230977817</v>
+        <v>0.9950909629754088</v>
       </c>
       <c r="H7" t="n">
         <v>4.06134E7</v>
       </c>
       <c r="I7" t="n">
-        <v>4.60073363460665E7</v>
+        <v>4.351450280816629E7</v>
       </c>
     </row>
     <row r="8">
@@ -3703,13 +3703,13 @@
       <c r="E8"/>
       <c r="F8"/>
       <c r="G8" t="n">
-        <v>0.9995345673308037</v>
+        <v>0.997724700484918</v>
       </c>
       <c r="H8" t="n">
         <v>5.41512E7</v>
       </c>
       <c r="I8" t="n">
-        <v>5.72795804217001E7</v>
+        <v>5.475825198565601E7</v>
       </c>
     </row>
     <row r="9">
@@ -3726,13 +3726,13 @@
       <c r="E9"/>
       <c r="F9"/>
       <c r="G9" t="n">
-        <v>0.9996457041113025</v>
+        <v>0.9987407415186009</v>
       </c>
       <c r="H9" t="n">
         <v>6.7689E7</v>
       </c>
       <c r="I9" t="n">
-        <v>9.545749562730536E7</v>
+        <v>9.673475833588755E7</v>
       </c>
     </row>
   </sheetData>
@@ -3792,16 +3792,16 @@
         <v>1.7328856E7</v>
       </c>
       <c r="F2" t="n">
-        <v>1278420.7322704357</v>
+        <v>2503154.8544669896</v>
       </c>
       <c r="G2" t="n">
-        <v>0.6285299502748479</v>
+        <v>0.5016568318185575</v>
       </c>
       <c r="H2" t="n">
         <v>0.0</v>
       </c>
       <c r="I2" t="n">
-        <v>2194833.919626999</v>
+        <v>2204750.61159843</v>
       </c>
     </row>
     <row r="3">
@@ -3818,13 +3818,13 @@
       <c r="E3"/>
       <c r="F3"/>
       <c r="G3" t="n">
-        <v>0.9536643388346006</v>
+        <v>0.8995192758252478</v>
       </c>
       <c r="H3" t="n">
         <v>6321402.0</v>
       </c>
       <c r="I3" t="n">
-        <v>9117420.615668638</v>
+        <v>9426485.396581534</v>
       </c>
     </row>
     <row r="4">
@@ -3841,13 +3841,13 @@
       <c r="E4"/>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>0.9918509334949751</v>
+        <v>0.9650290821275218</v>
       </c>
       <c r="H4" t="n">
         <v>1.404756E7</v>
       </c>
       <c r="I4" t="n">
-        <v>1.8103220857005727E7</v>
+        <v>1.790652372187222E7</v>
       </c>
     </row>
     <row r="5">
@@ -3864,13 +3864,13 @@
       <c r="E5"/>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>0.9974025405947167</v>
+        <v>0.9831445307180117</v>
       </c>
       <c r="H5" t="n">
         <v>2.34126E7</v>
       </c>
       <c r="I5" t="n">
-        <v>2.817298082713883E7</v>
+        <v>2.7181395560143452E7</v>
       </c>
     </row>
     <row r="6">
@@ -3887,13 +3887,13 @@
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6" t="n">
-        <v>0.9987111093773299</v>
+        <v>0.9906655119068448</v>
       </c>
       <c r="H6" t="n">
         <v>3.277764E7</v>
       </c>
       <c r="I6" t="n">
-        <v>3.7838721808961526E7</v>
+        <v>3.573574412286451E7</v>
       </c>
     </row>
     <row r="7">
@@ -3910,13 +3910,13 @@
       <c r="E7"/>
       <c r="F7"/>
       <c r="G7" t="n">
-        <v>0.9991858666261639</v>
+        <v>0.9946718352325162</v>
       </c>
       <c r="H7" t="n">
         <v>4.214268E7</v>
       </c>
       <c r="I7" t="n">
-        <v>4.7718463098498486E7</v>
+        <v>4.51488888804776E7</v>
       </c>
     </row>
     <row r="8">
@@ -3933,13 +3933,13 @@
       <c r="E8"/>
       <c r="F8"/>
       <c r="G8" t="n">
-        <v>0.9994746335245673</v>
+        <v>0.997435491413859</v>
       </c>
       <c r="H8" t="n">
         <v>5.619024E7</v>
       </c>
       <c r="I8" t="n">
-        <v>5.958356242265702E7</v>
+        <v>5.6920497953262776E7</v>
       </c>
     </row>
     <row r="9">
@@ -3956,13 +3956,13 @@
       <c r="E9"/>
       <c r="F9"/>
       <c r="G9" t="n">
-        <v>0.9995966265747721</v>
+        <v>0.9985523568318647</v>
       </c>
       <c r="H9" t="n">
         <v>7.02378E7</v>
       </c>
       <c r="I9" t="n">
-        <v>9.981011804738502E7</v>
+        <v>1.023091857878579E8</v>
       </c>
     </row>
   </sheetData>
@@ -4022,16 +4022,16 @@
         <v>1.75047685E7</v>
       </c>
       <c r="F2" t="n">
-        <v>1126660.8787417596</v>
+        <v>2776735.6691535655</v>
       </c>
       <c r="G2" t="n">
-        <v>0.645408164066837</v>
+        <v>0.4880844610998426</v>
       </c>
       <c r="H2" t="n">
         <v>0.0</v>
       </c>
       <c r="I2" t="n">
-        <v>2259219.3236311353</v>
+        <v>2343260.3551267567</v>
       </c>
     </row>
     <row r="3">
@@ -4048,13 +4048,13 @@
       <c r="E3"/>
       <c r="F3"/>
       <c r="G3" t="n">
-        <v>0.967016644636003</v>
+        <v>0.8901482187553638</v>
       </c>
       <c r="H3" t="n">
         <v>6513372.0</v>
       </c>
       <c r="I3" t="n">
-        <v>9316208.054378072</v>
+        <v>9664106.793198971</v>
       </c>
     </row>
     <row r="4">
@@ -4071,13 +4071,13 @@
       <c r="E4"/>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>0.9947112696748889</v>
+        <v>0.9614965487832644</v>
       </c>
       <c r="H4" t="n">
         <v>1.447416E7</v>
       </c>
       <c r="I4" t="n">
-        <v>1.873081245142932E7</v>
+        <v>1.8350933133591082E7</v>
       </c>
     </row>
     <row r="5">
@@ -4094,13 +4094,13 @@
       <c r="E5"/>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>0.9983861540356846</v>
+        <v>0.981392384595089</v>
       </c>
       <c r="H5" t="n">
         <v>2.41236E7</v>
       </c>
       <c r="I5" t="n">
-        <v>2.9256821426698666E7</v>
+        <v>2.7770386621754475E7</v>
       </c>
     </row>
     <row r="6">
@@ -4117,13 +4117,13 @@
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6" t="n">
-        <v>0.9992067304403369</v>
+        <v>0.9895204555261613</v>
       </c>
       <c r="H6" t="n">
         <v>3.377304E7</v>
       </c>
       <c r="I6" t="n">
-        <v>3.849816460867167E7</v>
+        <v>3.6516269701597296E7</v>
       </c>
     </row>
     <row r="7">
@@ -4140,13 +4140,13 @@
       <c r="E7"/>
       <c r="F7"/>
       <c r="G7" t="n">
-        <v>0.9994981938778568</v>
+        <v>0.9937053152116807</v>
       </c>
       <c r="H7" t="n">
         <v>4.342248E7</v>
       </c>
       <c r="I7" t="n">
-        <v>4.858069229864371E7</v>
+        <v>4.6256571848661646E7</v>
       </c>
     </row>
     <row r="8">
@@ -4163,13 +4163,13 @@
       <c r="E8"/>
       <c r="F8"/>
       <c r="G8" t="n">
-        <v>0.9996873994648944</v>
+        <v>0.9968728521031284</v>
       </c>
       <c r="H8" t="n">
         <v>5.789664E7</v>
       </c>
       <c r="I8" t="n">
-        <v>6.029571002421809E7</v>
+        <v>5.774834701793027E7</v>
       </c>
     </row>
     <row r="9">
@@ -4186,13 +4186,13 @@
       <c r="E9"/>
       <c r="F9"/>
       <c r="G9" t="n">
-        <v>0.9997752041108113</v>
+        <v>0.9983198292510981</v>
       </c>
       <c r="H9" t="n">
         <v>7.23708E7</v>
       </c>
       <c r="I9" t="n">
-        <v>1.0462860188931164E8</v>
+        <v>1.0198695503843799E8</v>
       </c>
     </row>
   </sheetData>
@@ -4252,16 +4252,16 @@
         <v>1.7680681E7</v>
       </c>
       <c r="F2" t="n">
-        <v>1236262.8596135199</v>
+        <v>3030570.5014007986</v>
       </c>
       <c r="G2" t="n">
-        <v>0.6409780822356334</v>
+        <v>0.4806440430659882</v>
       </c>
       <c r="H2" t="n">
         <v>0.0</v>
       </c>
       <c r="I2" t="n">
-        <v>2364215.3223594716</v>
+        <v>2459062.8034061044</v>
       </c>
     </row>
     <row r="3">
@@ -4278,13 +4278,13 @@
       <c r="E3"/>
       <c r="F3"/>
       <c r="G3" t="n">
-        <v>0.9623437015802728</v>
+        <v>0.8812971061465336</v>
       </c>
       <c r="H3" t="n">
         <v>6605064.0</v>
       </c>
       <c r="I3" t="n">
-        <v>9521981.18712221</v>
+        <v>9911760.854826286</v>
       </c>
     </row>
     <row r="4">
@@ -4301,13 +4301,13 @@
       <c r="E4"/>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>0.9935895568728377</v>
+        <v>0.9582821498787292</v>
       </c>
       <c r="H4" t="n">
         <v>1.467792E7</v>
       </c>
       <c r="I4" t="n">
-        <v>1.913051556642613E7</v>
+        <v>1.8913776014175884E7</v>
       </c>
     </row>
     <row r="5">
@@ -4324,13 +4324,13 @@
       <c r="E5"/>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>0.9980428355672499</v>
+        <v>0.9799046201896862</v>
       </c>
       <c r="H5" t="n">
         <v>2.44632E7</v>
       </c>
       <c r="I5" t="n">
-        <v>3.0041337138225403E7</v>
+        <v>2.8760870000713225E7</v>
       </c>
     </row>
     <row r="6">
@@ -4347,13 +4347,13 @@
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6" t="n">
-        <v>0.9990360099817422</v>
+        <v>0.9886675745125428</v>
       </c>
       <c r="H6" t="n">
         <v>3.424848E7</v>
       </c>
       <c r="I6" t="n">
-        <v>3.997703708373519E7</v>
+        <v>3.7835142976904556E7</v>
       </c>
     </row>
     <row r="7">
@@ -4370,13 +4370,13 @@
       <c r="E7"/>
       <c r="F7"/>
       <c r="G7" t="n">
-        <v>0.9993771167524599</v>
+        <v>0.9932811977095226</v>
       </c>
       <c r="H7" t="n">
         <v>4.403376E7</v>
       </c>
       <c r="I7" t="n">
-        <v>5.0307044028346926E7</v>
+        <v>4.792724933265311E7</v>
       </c>
     </row>
     <row r="8">
@@ -4393,13 +4393,13 @@
       <c r="E8"/>
       <c r="F8"/>
       <c r="G8" t="n">
-        <v>0.9995909659814574</v>
+        <v>0.9966956589511456</v>
       </c>
       <c r="H8" t="n">
         <v>5.871168E7</v>
       </c>
       <c r="I8" t="n">
-        <v>6.273894441016695E7</v>
+        <v>5.999830451554396E7</v>
       </c>
     </row>
     <row r="9">
@@ -4416,13 +4416,13 @@
       <c r="E9"/>
       <c r="F9"/>
       <c r="G9" t="n">
-        <v>0.9996900571872769</v>
+        <v>0.9981301625203237</v>
       </c>
       <c r="H9" t="n">
         <v>7.33896E7</v>
       </c>
       <c r="I9" t="n">
-        <v>1.0750902288336046E8</v>
+        <v>1.0536677930910586E8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>